<commit_message>
My Request Button event handling.
</commit_message>
<xml_diff>
--- a/Documents/ProcessFlow.xlsx
+++ b/Documents/ProcessFlow.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rautatul/Documents/Atul/Study/Projects/booking-dev/booking/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rautatul/Documents/Atul/Study/Projects/booking-dev-int/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBAEE1D1-5669-2744-9F4B-5C2473213A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A3AD79-9CB5-9241-9733-524CE8DE8C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="500" windowWidth="27640" windowHeight="15800" activeTab="1" xr2:uid="{90052BEC-FEBB-F247-ACB1-709744DE85BE}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t>Timeline</t>
   </si>
@@ -94,6 +94,42 @@
   </si>
   <si>
     <t>Customer Login</t>
+  </si>
+  <si>
+    <t>Accept Button</t>
+  </si>
+  <si>
+    <t>T_POST</t>
+  </si>
+  <si>
+    <t>SERVICE_PROVIDER</t>
+  </si>
+  <si>
+    <t>ACCEPTED</t>
+  </si>
+  <si>
+    <t>STARUS</t>
+  </si>
+  <si>
+    <t>Service Provider ID</t>
+  </si>
+  <si>
+    <t>Cancle</t>
+  </si>
+  <si>
+    <t>NEW</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>Close</t>
+  </si>
+  <si>
+    <t>CLOSED</t>
+  </si>
+  <si>
+    <t>Pune</t>
   </si>
 </sst>
 </file>
@@ -1681,6 +1717,119 @@
         <a:xfrm>
           <a:off x="1866900" y="6883400"/>
           <a:ext cx="431800" cy="431800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Oval 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E17D4139-ACC3-3346-AA1D-1891D2C925B4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6667500" y="1727200"/>
+          <a:ext cx="190500" cy="177800"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Graphic 8" descr="Marker">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8147CCB8-A9B4-C24F-9C45-93951B6D7F33}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId24"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6578600" y="1981200"/>
+          <a:ext cx="368300" cy="368300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8641,19 +8790,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00AD811D-9B4C-B744-B95C-0E48158B425D}">
-  <dimension ref="C3:AG31"/>
+  <dimension ref="C3:BX31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="AW17" sqref="AW17"/>
+      <selection activeCell="BX20" sqref="BX20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="63" max="63" width="11.5" customWidth="1"/>
     <col min="64" max="64" width="4.33203125" customWidth="1"/>
+    <col min="66" max="66" width="5.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:33" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:44" x14ac:dyDescent="0.2">
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
@@ -8664,12 +8814,81 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="3:44" x14ac:dyDescent="0.2">
+      <c r="AR10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="6:76" x14ac:dyDescent="0.2">
+      <c r="BK17" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="6:76" x14ac:dyDescent="0.2">
+      <c r="BN18" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="6:76" x14ac:dyDescent="0.2">
+      <c r="BO19" t="s">
+        <v>24</v>
+      </c>
+      <c r="BX19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="6:76" x14ac:dyDescent="0.2">
+      <c r="BO20" t="s">
+        <v>26</v>
+      </c>
+      <c r="BX20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="6:76" x14ac:dyDescent="0.2">
+      <c r="BK22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="BN22" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="6:76" x14ac:dyDescent="0.2">
+      <c r="BO23" t="s">
+        <v>24</v>
+      </c>
+      <c r="BX23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="6:76" x14ac:dyDescent="0.2">
+      <c r="BO24" t="s">
+        <v>26</v>
+      </c>
+      <c r="BX24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="6:76" x14ac:dyDescent="0.2">
+      <c r="BK26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="BN26" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="6:76" x14ac:dyDescent="0.2">
       <c r="G27" t="s">
         <v>11</v>
       </c>
+      <c r="BO27" t="s">
+        <v>26</v>
+      </c>
+      <c r="BX27" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="31" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="6:76" x14ac:dyDescent="0.2">
       <c r="F31" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Amount changes in Dashboard and My request Screen.
</commit_message>
<xml_diff>
--- a/Documents/ProcessFlow.xlsx
+++ b/Documents/ProcessFlow.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rautatul/Documents/Atul/Study/Projects/booking-dev-int/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A3AD79-9CB5-9241-9733-524CE8DE8C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E6CCAA-EE9E-7A4F-A0E9-F51A47615210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="500" windowWidth="27640" windowHeight="15800" activeTab="1" xr2:uid="{90052BEC-FEBB-F247-ACB1-709744DE85BE}"/>
+    <workbookView xWindow="780" yWindow="500" windowWidth="27640" windowHeight="15800" activeTab="4" xr2:uid="{90052BEC-FEBB-F247-ACB1-709744DE85BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
     <sheet name="Activity Process 1" sheetId="6" r:id="rId2"/>
     <sheet name="Activity Process 2" sheetId="9" r:id="rId3"/>
     <sheet name="DashboardLayout" sheetId="7" r:id="rId4"/>
+    <sheet name="PushNotification" sheetId="10" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -8379,6 +8380,1357 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="52" name="Rectangle 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{566C88EA-E588-334E-81D3-CCA773AEDE4B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2235200" y="889000"/>
+          <a:ext cx="7023100" cy="4864100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Can 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C6C797A-EDC3-BF44-8BE0-94917828E319}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2476500" y="1828800"/>
+          <a:ext cx="838200" cy="635000"/>
+        </a:xfrm>
+        <a:prstGeom prst="can">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>Fire base</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5D059A1-9772-5841-A86B-F19FCC4F2DC6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4038600" y="1536700"/>
+          <a:ext cx="1930400" cy="1231900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>Fire base Application</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED7DA4E2-9BD6-BD4D-A15D-B832B23F6E15}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="4"/>
+          <a:endCxn id="3" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3314700" y="2146300"/>
+          <a:ext cx="723900" cy="6350"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rectangle 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65115D2D-99E6-9B4C-9121-57A962D37147}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7759700" y="1308100"/>
+          <a:ext cx="622300" cy="1676400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>Mobile</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D38BC47-62F7-D040-9E12-8104957921D7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5283200" y="4165600"/>
+          <a:ext cx="1955800" cy="1282700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>Booking App</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2DBF6B0-5006-554E-B964-AEBF55EBCC6B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="7" idx="0"/>
+          <a:endCxn id="3" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="5969000" y="2152650"/>
+          <a:ext cx="292100" cy="2012950"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>641350</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{038F5262-6CED-0247-812D-DD394EE7EB59}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="6" idx="2"/>
+          <a:endCxn id="7" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6261100" y="2984500"/>
+          <a:ext cx="1809750" cy="1181100"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="Rectangle 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{053C617F-75EA-574A-B3B9-DBE5DF5DE6F4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4838700" y="1930400"/>
+          <a:ext cx="596900" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>Tokan</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="Straight Arrow Connector 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A494832-2997-474A-9C0F-2321FA46D783}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="2"/>
+          <a:endCxn id="7" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5003800" y="2768600"/>
+          <a:ext cx="1257300" cy="1397000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="32" name="Rectangle 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E42E65B-908A-704D-BB8E-ED7738AF0B70}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5397500" y="3200400"/>
+          <a:ext cx="596900" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>Tokan</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="33" name="Straight Arrow Connector 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38D92F42-B728-FA44-B364-9A9E5A0CDD79}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="7" idx="1"/>
+          <a:endCxn id="3" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="5003800" y="2768600"/>
+          <a:ext cx="279400" cy="2038350"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="36" name="Rectangle 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAE44D10-8652-E944-AD0D-E3B01F703510}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4597400" y="3594100"/>
+          <a:ext cx="762000" cy="482600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>Tokan</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>Message</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="41" name="Straight Arrow Connector 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{276CF1E5-24C4-CA46-B5EF-0406152598BF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="3"/>
+          <a:endCxn id="6" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5969000" y="2146300"/>
+          <a:ext cx="1790700" cy="6350"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="44" name="Rectangle 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B43B5EC-838D-9D4F-895C-6CD2C06772C2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6311900" y="1917700"/>
+          <a:ext cx="838200" cy="368300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>Message</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="53" name="Rectangle 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5A53E96-7821-384A-BF55-D66B43DD6A8E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11544300" y="2286000"/>
+          <a:ext cx="584200" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>MQTT</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="54" name="Straight Arrow Connector 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87517EF1-F33B-1147-906A-61F4F5740D7A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="6" idx="3"/>
+          <a:endCxn id="53" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8382000" y="2146300"/>
+          <a:ext cx="3162300" cy="330200"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="58" name="Straight Arrow Connector 57">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD6F8FD1-5788-F04D-BE19-61A40985C2E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="7" idx="3"/>
+          <a:endCxn id="53" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7239000" y="2667000"/>
+          <a:ext cx="4597400" cy="2139950"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="65" name="Rectangle 64">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD2A06F3-6BA2-8D47-B228-CE95F9B2E83C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9410700" y="3429000"/>
+          <a:ext cx="774700" cy="469900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>Topic</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>Message</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="66" name="Rectangle 65">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEDD18FB-920C-E846-B937-803B20C10764}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9550400" y="2146300"/>
+          <a:ext cx="774700" cy="317500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>Message</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="68" name="Multiply 67">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C9949F8-246F-4540-BCC0-1C5AC7A13501}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8483600" y="4025900"/>
+          <a:ext cx="292100" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="mathMultiply">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="69" name="Multiply 68">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C23CF7BB-3BF4-6A41-BF67-58C63AA27350}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8890000" y="2070100"/>
+          <a:ext cx="292100" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="mathMultiply">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -8792,7 +10144,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00AD811D-9B4C-B744-B95C-0E48158B425D}">
   <dimension ref="C3:BX31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="BX20" sqref="BX20"/>
     </sheetView>
   </sheetViews>
@@ -8971,4 +10323,19 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28660E41-670A-654D-9A2B-91995503F4ED}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>